<commit_message>
with final svm linear results
</commit_message>
<xml_diff>
--- a/output/tuning/aggregate-metrics.xlsx
+++ b/output/tuning/aggregate-metrics.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27217"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabio\Documents\GitHub\best-answer-prediction\output\tuning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/git/bap-script/output/tuning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="7755" firstSheet="14" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="nb" sheetId="1" r:id="rId1"/>
@@ -39,12 +39,20 @@
     <sheet name="C5.0" sheetId="26" r:id="rId25"/>
     <sheet name="xgbTree" sheetId="27" r:id="rId26"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="1402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="1410">
   <si>
     <t>AUROC</t>
   </si>
@@ -4250,12 +4258,36 @@
   </si>
   <si>
     <t>0.8366989</t>
+  </si>
+  <si>
+    <t>0.6738916</t>
+  </si>
+  <si>
+    <t>0.6634969</t>
+  </si>
+  <si>
+    <t>0.6317431</t>
+  </si>
+  <si>
+    <t>0.6152986</t>
+  </si>
+  <si>
+    <t>0.66418</t>
+  </si>
+  <si>
+    <t>0.6562967</t>
+  </si>
+  <si>
+    <t>0.6340334</t>
+  </si>
+  <si>
+    <t>0.6281851</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4356,9 +4388,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -4386,31 +4418,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -4438,23 +4453,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4637,9 +4635,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4662,7 +4660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4688,7 +4686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4714,7 +4712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -4740,7 +4738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4766,7 +4764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -4792,7 +4790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -4818,7 +4816,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -4844,7 +4842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -4870,7 +4868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -4896,7 +4894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -4922,7 +4920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -4945,7 +4943,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -4968,7 +4966,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4991,7 +4989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -5014,7 +5012,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -5037,7 +5035,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -5058,9 +5056,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5083,7 +5081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5109,7 +5107,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5135,7 +5133,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -5161,7 +5159,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -5187,7 +5185,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -5213,7 +5211,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -5239,7 +5237,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -5265,7 +5263,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -5291,7 +5289,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -5317,7 +5315,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -5343,7 +5341,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -5366,7 +5364,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -5389,7 +5387,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -5412,7 +5410,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -5435,7 +5433,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -5458,7 +5456,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -5479,9 +5477,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5504,7 +5502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5530,7 +5528,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5556,7 +5554,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -5582,7 +5580,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -5608,7 +5606,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -5634,7 +5632,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -5660,7 +5658,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -5686,7 +5684,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -5712,7 +5710,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -5738,7 +5736,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -5764,7 +5762,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -5787,7 +5785,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -5810,7 +5808,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -5833,7 +5831,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -5856,7 +5854,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -5879,7 +5877,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -5900,9 +5898,9 @@
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5925,7 +5923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5951,7 +5949,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -5977,7 +5975,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -6003,7 +6001,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -6029,7 +6027,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -6055,7 +6053,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -6081,7 +6079,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -6107,7 +6105,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -6133,7 +6131,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -6159,7 +6157,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -6185,7 +6183,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -6208,7 +6206,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -6231,7 +6229,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -6254,7 +6252,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -6277,7 +6275,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -6300,7 +6298,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -6321,9 +6319,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6346,7 +6344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6372,7 +6370,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6398,7 +6396,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -6424,7 +6422,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -6450,7 +6448,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -6476,7 +6474,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -6502,7 +6500,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -6528,7 +6526,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -6554,7 +6552,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -6580,7 +6578,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -6606,7 +6604,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -6629,7 +6627,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -6652,7 +6650,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -6675,7 +6673,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -6698,7 +6696,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -6721,7 +6719,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -6729,52 +6727,52 @@
         <v>623</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>1326</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>1327</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>1325</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>1324</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>1323</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>1322</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>1321</v>
       </c>
@@ -6792,9 +6790,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6817,7 +6815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6843,7 +6841,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6869,7 +6867,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -6895,7 +6893,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -6921,7 +6919,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -6947,7 +6945,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -6973,7 +6971,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -6999,7 +6997,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -7025,7 +7023,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -7051,7 +7049,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -7077,7 +7075,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -7100,7 +7098,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -7123,7 +7121,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -7146,7 +7144,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -7169,7 +7167,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -7192,7 +7190,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -7213,9 +7211,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7238,7 +7236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7264,7 +7262,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -7290,7 +7288,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -7316,7 +7314,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -7342,7 +7340,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -7368,7 +7366,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -7394,7 +7392,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -7420,7 +7418,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -7446,7 +7444,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -7472,7 +7470,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -7498,7 +7496,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -7521,7 +7519,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -7544,7 +7542,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -7567,7 +7565,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -7590,7 +7588,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -7613,7 +7611,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -7634,12 +7632,12 @@
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7662,7 +7660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7688,7 +7686,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -7714,7 +7712,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -7740,7 +7738,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -7766,7 +7764,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -7792,7 +7790,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -7818,7 +7816,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -7844,7 +7842,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -7870,7 +7868,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -7896,7 +7894,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -7922,7 +7920,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -7945,7 +7943,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -7968,7 +7966,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -7991,7 +7989,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -8014,7 +8012,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -8037,7 +8035,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -8056,9 +8054,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8081,7 +8079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -8107,7 +8105,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8133,7 +8131,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -8159,7 +8157,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -8185,7 +8183,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -8211,7 +8209,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -8237,7 +8235,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -8263,7 +8261,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -8289,7 +8287,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -8315,7 +8313,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -8341,7 +8339,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -8364,7 +8362,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -8387,7 +8385,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -8410,7 +8408,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -8433,7 +8431,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -8456,7 +8454,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -8473,11 +8471,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8500,7 +8500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -8526,12 +8526,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="C3" t="s">
         <v>420</v>
@@ -8552,12 +8552,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>843</v>
+        <v>1402</v>
       </c>
       <c r="C4" t="s">
         <v>420</v>
@@ -8578,12 +8578,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>843</v>
+        <v>1403</v>
       </c>
       <c r="C5" t="s">
         <v>420</v>
@@ -8604,12 +8604,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>843</v>
+        <v>1404</v>
       </c>
       <c r="C6" t="s">
         <v>420</v>
@@ -8630,12 +8630,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>846</v>
+        <v>1405</v>
       </c>
       <c r="C7" t="s">
         <v>847</v>
@@ -8656,12 +8656,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>846</v>
+        <v>1406</v>
       </c>
       <c r="C8" t="s">
         <v>847</v>
@@ -8682,12 +8682,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>846</v>
+        <v>1407</v>
       </c>
       <c r="C9" t="s">
         <v>847</v>
@@ -8708,12 +8708,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>846</v>
+        <v>1408</v>
       </c>
       <c r="C10" t="s">
         <v>847</v>
@@ -8734,12 +8734,12 @@
         <v>845</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>846</v>
+        <v>1409</v>
       </c>
       <c r="C11" t="s">
         <v>847</v>
@@ -8760,7 +8760,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -8806,7 +8806,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -8852,7 +8852,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -8896,9 +8896,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -8999,7 +8999,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -9204,7 +9204,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -9227,7 +9227,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -9317,9 +9317,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9342,7 +9342,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9394,7 +9394,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -9420,7 +9420,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -9446,7 +9446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -9472,7 +9472,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -9550,7 +9550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -9576,7 +9576,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -9671,7 +9671,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -9717,7 +9717,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -9738,9 +9738,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -9789,7 +9789,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -9867,7 +9867,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -9893,7 +9893,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -9919,7 +9919,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -9945,7 +9945,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -10069,7 +10069,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -10115,7 +10115,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -10138,7 +10138,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -10159,9 +10159,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -10210,7 +10210,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -10236,7 +10236,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -10262,7 +10262,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10288,7 +10288,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -10340,7 +10340,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -10392,7 +10392,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -10418,7 +10418,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -10444,7 +10444,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -10467,7 +10467,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -10490,7 +10490,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -10513,7 +10513,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -10536,7 +10536,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -10559,7 +10559,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -10580,9 +10580,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10605,7 +10605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -10631,7 +10631,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -10709,7 +10709,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -10735,7 +10735,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -10761,7 +10761,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -10787,7 +10787,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -10813,7 +10813,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -10839,7 +10839,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -10865,7 +10865,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -10911,7 +10911,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -10934,7 +10934,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -10957,7 +10957,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -10980,7 +10980,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -11001,9 +11001,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11026,7 +11026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -11078,7 +11078,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -11104,7 +11104,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -11182,7 +11182,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -11208,7 +11208,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -11234,7 +11234,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -11260,7 +11260,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -11286,7 +11286,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -11332,7 +11332,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -11401,7 +11401,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -11422,9 +11422,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11447,7 +11447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -11473,7 +11473,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -11499,7 +11499,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -11525,7 +11525,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -11551,7 +11551,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -11577,7 +11577,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -11603,7 +11603,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -11629,7 +11629,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -11655,7 +11655,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -11681,7 +11681,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -11730,7 +11730,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -11753,7 +11753,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -11776,7 +11776,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -11799,7 +11799,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -11822,7 +11822,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -11843,9 +11843,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11868,7 +11868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -11894,7 +11894,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -11920,7 +11920,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -11972,7 +11972,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -11998,7 +11998,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -12024,7 +12024,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -12050,7 +12050,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -12076,7 +12076,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -12102,7 +12102,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -12128,7 +12128,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -12151,7 +12151,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -12174,7 +12174,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -12197,7 +12197,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -12220,7 +12220,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -12260,16 +12260,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12292,7 +12292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -12318,7 +12318,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -12344,7 +12344,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -12370,7 +12370,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -12396,7 +12396,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -12422,7 +12422,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -12448,7 +12448,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -12474,7 +12474,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -12500,7 +12500,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -12526,7 +12526,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -12552,7 +12552,7 @@
         <v>1221</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -12598,7 +12598,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -12621,7 +12621,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -12644,7 +12644,7 @@
         <v>1255</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -12667,7 +12667,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -12688,9 +12688,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12713,7 +12713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -12739,7 +12739,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -12765,7 +12765,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -12791,7 +12791,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -12817,7 +12817,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -12843,7 +12843,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -12895,7 +12895,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -12921,7 +12921,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -12973,7 +12973,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -12996,7 +12996,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -13019,7 +13019,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -13042,7 +13042,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -13065,7 +13065,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -13088,7 +13088,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -13109,12 +13109,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13137,7 +13137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -13189,7 +13189,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -13215,7 +13215,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -13267,7 +13267,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -13293,7 +13293,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -13345,7 +13345,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -13397,7 +13397,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -13420,7 +13420,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -13443,7 +13443,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -13466,7 +13466,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -13489,7 +13489,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -13512,7 +13512,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -13533,9 +13533,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13558,7 +13558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -13584,7 +13584,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -13610,7 +13610,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -13636,7 +13636,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -13662,7 +13662,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -13688,7 +13688,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -13714,7 +13714,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -13740,7 +13740,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -13766,7 +13766,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -13792,7 +13792,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -13818,7 +13818,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -13864,7 +13864,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -13887,7 +13887,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -13910,7 +13910,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -13933,7 +13933,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -13954,9 +13954,9 @@
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13979,7 +13979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -14005,7 +14005,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -14031,7 +14031,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -14057,7 +14057,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -14083,7 +14083,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -14109,7 +14109,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -14135,7 +14135,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -14161,7 +14161,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -14187,7 +14187,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -14213,7 +14213,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -14239,7 +14239,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -14262,7 +14262,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -14285,7 +14285,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -14308,7 +14308,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -14331,7 +14331,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -14354,7 +14354,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -14375,9 +14375,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14400,7 +14400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -14426,7 +14426,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -14452,7 +14452,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -14478,7 +14478,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -14504,7 +14504,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -14530,7 +14530,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -14556,7 +14556,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -14582,7 +14582,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -14608,7 +14608,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -14634,7 +14634,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -14660,7 +14660,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -14683,7 +14683,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -14706,7 +14706,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -14752,7 +14752,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -14794,9 +14794,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14819,7 +14819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -14845,7 +14845,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -14871,7 +14871,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -14897,7 +14897,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -14923,7 +14923,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -14949,7 +14949,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -14975,7 +14975,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -15001,7 +15001,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -15027,7 +15027,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -15053,7 +15053,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -15102,7 +15102,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -15125,7 +15125,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -15148,7 +15148,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -15171,7 +15171,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -15194,7 +15194,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -15215,9 +15215,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15240,7 +15240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -15266,7 +15266,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -15292,7 +15292,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -15318,7 +15318,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -15344,7 +15344,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -15370,7 +15370,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -15396,7 +15396,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -15422,7 +15422,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -15448,7 +15448,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -15474,7 +15474,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -15500,7 +15500,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -15546,7 +15546,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -15569,7 +15569,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -15592,7 +15592,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -15615,7 +15615,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>

</xml_diff>